<commit_message>
Last minute changes to schematic before the layout begins
</commit_message>
<xml_diff>
--- a/Schematics/Board_Layout_Checklist.xlsx
+++ b/Schematics/Board_Layout_Checklist.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
   <si>
     <t>Item</t>
   </si>
@@ -64,6 +64,12 @@
   </si>
   <si>
     <t>Any generic I/O pin can be used for LCD back light</t>
+  </si>
+  <si>
+    <t>check</t>
+  </si>
+  <si>
+    <t>used PB6</t>
   </si>
 </sst>
 </file>
@@ -417,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:B17"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -428,7 +434,7 @@
     <col min="1" max="1" width="64.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -436,64 +442,97 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:2" s="2" customFormat="1" ht="130.5" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
made some updates to the layout checklist
</commit_message>
<xml_diff>
--- a/Schematics/Board_Layout_Checklist.xlsx
+++ b/Schematics/Board_Layout_Checklist.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
   <si>
     <t>Item</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>used PB6</t>
+  </si>
+  <si>
+    <t>External Oscilloscope</t>
   </si>
 </sst>
 </file>
@@ -423,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,15 +538,20 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:2" s="2" customFormat="1" ht="130.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" s="2" customFormat="1" ht="130.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="3"/>
+      <c r="B18" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>

</xml_diff>